<commit_message>
content+ system to progress through content
</commit_message>
<xml_diff>
--- a/src/assets/narrative/A1_A2.xlsx
+++ b/src/assets/narrative/A1_A2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schne\GitHub\run-it-again\src\assets\narrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1612CCD9-D468-4554-85EF-2D6BBD1AC6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB375F6-F3D5-4FD6-A8D6-33988435A42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{897B4BAE-C0FB-437A-8E6A-40B4B514A057}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t>Code</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>DECISION</t>
+  </si>
+  <si>
+    <t>Unique</t>
   </si>
 </sst>
 </file>
@@ -608,7 +611,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,8 +762,8 @@
       <c r="E11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>7</v>
+      <c r="F11" s="4">
+        <v>-100</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -826,6 +829,14 @@
         <v>26</v>
       </c>
       <c r="F17" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>